<commit_message>
up to date 2019-06-03
</commit_message>
<xml_diff>
--- a/templates/PE&PA_waterSamplesTemplate_DONOTSAVE.xlsx
+++ b/templates/PE&PA_waterSamplesTemplate_DONOTSAVE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brittnibertolet/OneDrive - nd.edu/underc-field-2019/data/gc2019underc/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\Documents\Summer2019\Limno\gc2019underc\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="11_D5860AFCDDD810671351515E592EDFA073F66C1B" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{64768B40-E8E9-D748-BFE9-F510AF4D0906}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A9316B-DCE0-4A94-B471-C6EDC09FF689}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="22420" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExampleRunFile" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="34">
   <si>
     <t>projectID</t>
   </si>
@@ -995,34 +996,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R58"/>
+  <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O58"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1078,10 +1079,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>34</v>
-      </c>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -1132,21 +1130,12 @@
         <v>1_19052201</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>34</v>
-      </c>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
-      </c>
-      <c r="D3" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E3" s="2">
-        <v>43607</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -1182,25 +1171,16 @@
         <v>19052201</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q40" si="0">CONCATENATE(O3,"_",P3)</f>
+        <f t="shared" ref="Q3:Q39" si="0">CONCATENATE(O3,"_",P3)</f>
         <v>2_19052201</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>34</v>
-      </c>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E4" s="2">
-        <v>43607</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
@@ -1240,21 +1220,12 @@
         <v>3_19052201</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>34</v>
-      </c>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E5" s="2">
-        <v>43607</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
@@ -1294,21 +1265,12 @@
         <v>4_19052201</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>34</v>
-      </c>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E6" s="2">
-        <v>43607</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
@@ -1348,21 +1310,12 @@
         <v>5_19052201</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>34</v>
-      </c>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E7" s="2">
-        <v>43607</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
@@ -1402,21 +1355,12 @@
         <v>6_19052201</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>34</v>
-      </c>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
-      </c>
-      <c r="D8" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E8" s="2">
-        <v>43607</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -1456,21 +1400,12 @@
         <v>7_19052201</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>34</v>
-      </c>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
-      </c>
-      <c r="D9" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E9" s="2">
-        <v>43607</v>
       </c>
       <c r="F9" t="s">
         <v>32</v>
@@ -1507,21 +1442,12 @@
         <v>8_19052201</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>34</v>
-      </c>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
-      </c>
-      <c r="D10" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E10" s="2">
-        <v>43607</v>
       </c>
       <c r="F10" t="s">
         <v>32</v>
@@ -1558,33 +1484,26 @@
         <v>9_19052201</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E11" s="2">
-        <v>43607</v>
-      </c>
-      <c r="F11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" t="s">
-        <v>32</v>
+    <row r="11" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="J11" s="2">
         <v>43607</v>
@@ -1595,46 +1514,42 @@
       <c r="L11" s="1">
         <v>43607</v>
       </c>
-      <c r="N11" t="s">
+      <c r="M11" s="5">
+        <v>1</v>
+      </c>
+      <c r="N11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P11">
         <v>19052201</v>
       </c>
-      <c r="Q11" t="str">
-        <f t="shared" si="0"/>
-        <v>10_19052201</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
-        <v>34</v>
-      </c>
+      <c r="Q11" s="4" t="str">
+        <f t="shared" ref="Q11:Q19" si="1">CONCATENATE(O11,"_",P11)</f>
+        <v>11_19052201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E12" s="2">
-        <v>43607</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="5">
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="4">
         <v>0</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="4">
         <v>0</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J12" s="2">
@@ -1646,49 +1561,42 @@
       <c r="L12" s="1">
         <v>43607</v>
       </c>
-      <c r="M12" s="5">
-        <v>1</v>
+      <c r="M12" s="4">
+        <v>2</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P12">
         <v>19052201</v>
       </c>
       <c r="Q12" s="4" t="str">
-        <f t="shared" ref="Q12:Q20" si="1">CONCATENATE(O12,"_",P12)</f>
-        <v>11_19052201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
-        <v>34</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>12_19052201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E13" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="4">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="H13" s="4">
-        <v>0</v>
-      </c>
-      <c r="I13" s="4" t="s">
+        <v>3.5</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="J13" s="2">
@@ -1701,38 +1609,31 @@
         <v>43607</v>
       </c>
       <c r="M13" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P13">
         <v>19052201</v>
       </c>
       <c r="Q13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>12_19052201</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
-        <v>34</v>
-      </c>
+        <v>13_19052201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E14" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
       <c r="F14" s="4" t="s">
         <v>18</v>
       </c>
@@ -1742,7 +1643,7 @@
       <c r="H14" s="4">
         <v>3.5</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J14" s="2">
@@ -1755,48 +1656,41 @@
         <v>43607</v>
       </c>
       <c r="M14" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P14">
         <v>19052201</v>
       </c>
       <c r="Q14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>13_19052201</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
-        <v>34</v>
-      </c>
+        <v>14_19052201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E15" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
       <c r="F15" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="4">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="H15" s="4">
-        <v>3.5</v>
-      </c>
-      <c r="I15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="5" t="s">
         <v>21</v>
       </c>
       <c r="J15" s="2">
@@ -1809,38 +1703,31 @@
         <v>43607</v>
       </c>
       <c r="M15" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P15">
         <v>19052201</v>
       </c>
       <c r="Q15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>14_19052201</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
-        <v>34</v>
-      </c>
+        <v>15_19052201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E16" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
       <c r="F16" s="4" t="s">
         <v>18</v>
       </c>
@@ -1850,7 +1737,7 @@
       <c r="H16" s="4">
         <v>6</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J16" s="2">
@@ -1863,48 +1750,41 @@
         <v>43607</v>
       </c>
       <c r="M16" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P16">
         <v>19052201</v>
       </c>
       <c r="Q16" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>15_19052201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
-        <v>34</v>
-      </c>
+        <v>16_19052201</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E17" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
       <c r="F17" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H17" s="4">
-        <v>6</v>
-      </c>
-      <c r="I17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="J17" s="2">
@@ -1917,38 +1797,31 @@
         <v>43607</v>
       </c>
       <c r="M17" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P17">
         <v>19052201</v>
       </c>
       <c r="Q17" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>16_19052201</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
-        <v>34</v>
-      </c>
+        <v>17_19052201</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E18" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
       <c r="F18" s="4" t="s">
         <v>18</v>
       </c>
@@ -1958,7 +1831,7 @@
       <c r="H18" s="4">
         <v>9</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J18" s="2">
@@ -1971,48 +1844,41 @@
         <v>43607</v>
       </c>
       <c r="M18" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P18">
         <v>19052201</v>
       </c>
       <c r="Q18" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>17_19052201</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
-        <v>34</v>
-      </c>
+        <v>18_19052201</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E19" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2"/>
       <c r="F19" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G19" s="4">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H19" s="4">
-        <v>9</v>
-      </c>
-      <c r="I19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="5" t="s">
         <v>21</v>
       </c>
       <c r="J19" s="2">
@@ -2025,48 +1891,41 @@
         <v>43607</v>
       </c>
       <c r="M19" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P19">
         <v>19052201</v>
       </c>
       <c r="Q19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>18_19052201</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>34</v>
-      </c>
+        <v>19_19052201</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E20" s="2">
-        <v>43607</v>
-      </c>
+      <c r="C20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2"/>
       <c r="F20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="5">
         <v>11</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="5">
         <v>11</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J20" s="2">
@@ -2078,49 +1937,42 @@
       <c r="L20" s="1">
         <v>43607</v>
       </c>
-      <c r="M20" s="4">
-        <v>1</v>
+      <c r="M20" s="5">
+        <v>2</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P20">
         <v>19052201</v>
       </c>
       <c r="Q20" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>19_19052201</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
-        <v>34</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>20_19052201</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E21" s="2">
-        <v>43607</v>
-      </c>
+      <c r="C21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="2"/>
       <c r="F21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="5">
-        <v>11</v>
-      </c>
-      <c r="H21" s="5">
-        <v>11</v>
-      </c>
-      <c r="I21" s="4" t="s">
+      <c r="G21" s="4">
+        <v>13</v>
+      </c>
+      <c r="H21" s="4">
+        <v>13</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>21</v>
       </c>
       <c r="J21" s="2">
@@ -2132,39 +1984,32 @@
       <c r="L21" s="1">
         <v>43607</v>
       </c>
-      <c r="M21" s="5">
-        <v>2</v>
+      <c r="M21" s="4">
+        <v>1</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P21">
         <v>19052201</v>
       </c>
       <c r="Q21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>20_19052201</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
-        <v>34</v>
-      </c>
+        <v>21_19052201</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E22" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="2"/>
       <c r="F22" s="4" t="s">
         <v>18</v>
       </c>
@@ -2174,7 +2019,7 @@
       <c r="H22" s="4">
         <v>13</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J22" s="2">
@@ -2187,48 +2032,41 @@
         <v>43607</v>
       </c>
       <c r="M22" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P22">
         <v>19052201</v>
       </c>
       <c r="Q22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>21_19052201</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
-        <v>34</v>
-      </c>
+        <v>22_19052201</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E23" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="2"/>
       <c r="F23" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G23" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H23" s="4">
-        <v>13</v>
-      </c>
-      <c r="I23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>21</v>
       </c>
       <c r="J23" s="2">
@@ -2241,38 +2079,31 @@
         <v>43607</v>
       </c>
       <c r="M23" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N23" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P23">
         <v>19052201</v>
       </c>
       <c r="Q23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>22_19052201</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
-        <v>34</v>
-      </c>
+        <v>23_19052201</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E24" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="2"/>
       <c r="F24" s="4" t="s">
         <v>18</v>
       </c>
@@ -2282,7 +2113,7 @@
       <c r="H24" s="4">
         <v>15</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J24" s="2">
@@ -2295,48 +2126,41 @@
         <v>43607</v>
       </c>
       <c r="M24" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P24">
         <v>19052201</v>
       </c>
       <c r="Q24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>23_19052201</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
-        <v>34</v>
-      </c>
+        <v>24_19052201</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E25" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="2"/>
       <c r="F25" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G25" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H25" s="4">
-        <v>15</v>
-      </c>
-      <c r="I25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="5" t="s">
         <v>21</v>
       </c>
       <c r="J25" s="2">
@@ -2349,38 +2173,31 @@
         <v>43607</v>
       </c>
       <c r="M25" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P25">
         <v>19052201</v>
       </c>
       <c r="Q25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>24_19052201</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
-        <v>34</v>
-      </c>
+        <v>25_19052201</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E26" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="2"/>
       <c r="F26" s="4" t="s">
         <v>18</v>
       </c>
@@ -2390,7 +2207,7 @@
       <c r="H26" s="4">
         <v>16</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J26" s="2">
@@ -2403,49 +2220,42 @@
         <v>43607</v>
       </c>
       <c r="M26" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P26">
         <v>19052201</v>
       </c>
       <c r="Q26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>25_19052201</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
-        <v>34</v>
-      </c>
+        <v>26_19052201</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E27" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="2"/>
       <c r="F27" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G27" s="4">
-        <v>16</v>
+        <v>3.5</v>
       </c>
       <c r="H27" s="4">
-        <v>16</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>21</v>
+        <v>3.5</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="J27" s="2">
         <v>43607</v>
@@ -2457,38 +2267,31 @@
         <v>43607</v>
       </c>
       <c r="M27" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O27">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P27">
         <v>19052201</v>
       </c>
       <c r="Q27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>26_19052201</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
-        <v>34</v>
-      </c>
+        <v>27_19052201</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E28" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="2"/>
       <c r="F28" s="4" t="s">
         <v>18</v>
       </c>
@@ -2498,7 +2301,7 @@
       <c r="H28" s="4">
         <v>3.5</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="4" t="s">
         <v>30</v>
       </c>
       <c r="J28" s="2">
@@ -2511,48 +2314,41 @@
         <v>43607</v>
       </c>
       <c r="M28" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O28">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P28">
         <v>19052201</v>
       </c>
       <c r="Q28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>27_19052201</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
-        <v>34</v>
-      </c>
+        <v>28_19052201</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E29" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="2"/>
       <c r="F29" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G29" s="4">
-        <v>3.5</v>
+        <v>13</v>
       </c>
       <c r="H29" s="4">
-        <v>3.5</v>
-      </c>
-      <c r="I29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J29" s="2">
@@ -2565,38 +2361,31 @@
         <v>43607</v>
       </c>
       <c r="M29" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O29">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P29">
         <v>19052201</v>
       </c>
       <c r="Q29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>28_19052201</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
-        <v>34</v>
-      </c>
+        <v>29_19052201</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E30" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="2"/>
       <c r="F30" s="4" t="s">
         <v>18</v>
       </c>
@@ -2606,7 +2395,7 @@
       <c r="H30" s="4">
         <v>13</v>
       </c>
-      <c r="I30" s="5" t="s">
+      <c r="I30" s="4" t="s">
         <v>30</v>
       </c>
       <c r="J30" s="2">
@@ -2619,49 +2408,42 @@
         <v>43607</v>
       </c>
       <c r="M30" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>31</v>
       </c>
       <c r="O30">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P30">
         <v>19052201</v>
       </c>
       <c r="Q30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>29_19052201</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
-        <v>34</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E31" s="2">
-        <v>43607</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="4">
-        <v>13</v>
-      </c>
-      <c r="H31" s="4">
-        <v>13</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>30</v>
+        <v>30_19052201</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="7">
+        <v>0</v>
+      </c>
+      <c r="H31" s="7">
+        <v>0</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="J31" s="2">
         <v>43607</v>
@@ -2672,49 +2454,42 @@
       <c r="L31" s="1">
         <v>43607</v>
       </c>
-      <c r="M31" s="4">
-        <v>2</v>
-      </c>
-      <c r="N31" s="4" t="s">
+      <c r="M31" s="7">
+        <v>1</v>
+      </c>
+      <c r="N31" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O31">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P31">
         <v>19052201</v>
       </c>
-      <c r="Q31" s="4" t="str">
+      <c r="Q31" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>30_19052201</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6">
-        <v>34</v>
-      </c>
+        <v>31_19052201</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E32" s="2">
-        <v>43607</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" s="7">
+      <c r="C32" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="6">
         <v>0</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="6">
         <v>0</v>
       </c>
-      <c r="I32" s="7" t="s">
+      <c r="I32" s="6" t="s">
         <v>21</v>
       </c>
       <c r="J32" s="2">
@@ -2726,49 +2501,42 @@
       <c r="L32" s="1">
         <v>43607</v>
       </c>
-      <c r="M32" s="7">
-        <v>1</v>
+      <c r="M32" s="6">
+        <v>2</v>
       </c>
       <c r="N32" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O32">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P32">
         <v>19052201</v>
       </c>
       <c r="Q32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>31_19052201</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6">
-        <v>34</v>
-      </c>
+        <v>32_19052201</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E33" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="2"/>
       <c r="F33" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G33" s="6">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="H33" s="6">
-        <v>0</v>
-      </c>
-      <c r="I33" s="6" t="s">
+        <v>2.5</v>
+      </c>
+      <c r="I33" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J33" s="2">
@@ -2781,38 +2549,31 @@
         <v>43607</v>
       </c>
       <c r="M33" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N33" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O33">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P33">
         <v>19052201</v>
       </c>
       <c r="Q33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>32_19052201</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="6">
-        <v>34</v>
-      </c>
+        <v>33_19052201</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E34" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="2"/>
       <c r="F34" s="6" t="s">
         <v>18</v>
       </c>
@@ -2822,7 +2583,7 @@
       <c r="H34" s="6">
         <v>2.5</v>
       </c>
-      <c r="I34" s="7" t="s">
+      <c r="I34" s="6" t="s">
         <v>21</v>
       </c>
       <c r="J34" s="2">
@@ -2835,48 +2596,41 @@
         <v>43607</v>
       </c>
       <c r="M34" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N34" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O34">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P34">
         <v>19052201</v>
       </c>
       <c r="Q34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>33_19052201</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6">
-        <v>34</v>
-      </c>
+        <v>34_19052201</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E35" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="2"/>
       <c r="F35" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G35" s="6">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="H35" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="I35" s="6" t="s">
+        <v>4.5</v>
+      </c>
+      <c r="I35" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J35" s="2">
@@ -2889,38 +2643,31 @@
         <v>43607</v>
       </c>
       <c r="M35" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N35" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O35">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P35">
         <v>19052201</v>
       </c>
       <c r="Q35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>34_19052201</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6">
-        <v>34</v>
-      </c>
+        <v>35_19052201</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E36" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="2"/>
       <c r="F36" s="6" t="s">
         <v>18</v>
       </c>
@@ -2930,7 +2677,7 @@
       <c r="H36" s="6">
         <v>4.5</v>
       </c>
-      <c r="I36" s="7" t="s">
+      <c r="I36" s="6" t="s">
         <v>21</v>
       </c>
       <c r="J36" s="2">
@@ -2943,48 +2690,41 @@
         <v>43607</v>
       </c>
       <c r="M36" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N36" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O36">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P36">
         <v>19052201</v>
       </c>
       <c r="Q36" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>35_19052201</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="6">
-        <v>34</v>
-      </c>
+        <v>36_19052201</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E37" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="2"/>
       <c r="F37" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G37" s="6">
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="H37" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="I37" s="6" t="s">
+        <v>6.5</v>
+      </c>
+      <c r="I37" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J37" s="2">
@@ -2997,38 +2737,31 @@
         <v>43607</v>
       </c>
       <c r="M37" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N37" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O37">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P37">
         <v>19052201</v>
       </c>
       <c r="Q37" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>36_19052201</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6">
-        <v>34</v>
-      </c>
+        <v>37_19052201</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E38" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="2"/>
       <c r="F38" s="6" t="s">
         <v>18</v>
       </c>
@@ -3038,7 +2771,7 @@
       <c r="H38" s="6">
         <v>6.5</v>
       </c>
-      <c r="I38" s="7" t="s">
+      <c r="I38" s="6" t="s">
         <v>21</v>
       </c>
       <c r="J38" s="2">
@@ -3051,48 +2784,41 @@
         <v>43607</v>
       </c>
       <c r="M38" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N38" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O38">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P38">
         <v>19052201</v>
       </c>
       <c r="Q38" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>37_19052201</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="6">
-        <v>34</v>
-      </c>
+        <v>38_19052201</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D39" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E39" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="2"/>
       <c r="F39" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G39" s="6">
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="H39" s="6">
-        <v>6.5</v>
-      </c>
-      <c r="I39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I39" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J39" s="2">
@@ -3105,48 +2831,41 @@
         <v>43607</v>
       </c>
       <c r="M39" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N39" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O39">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P39">
         <v>19052201</v>
       </c>
       <c r="Q39" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>38_19052201</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="6">
-        <v>34</v>
-      </c>
+        <v>39_19052201</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E40" s="2">
-        <v>43607</v>
-      </c>
+      <c r="C40" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="2"/>
       <c r="F40" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G40" s="7">
         <v>8</v>
       </c>
-      <c r="H40" s="6">
+      <c r="H40" s="7">
         <v>8</v>
       </c>
-      <c r="I40" s="7" t="s">
+      <c r="I40" s="6" t="s">
         <v>21</v>
       </c>
       <c r="J40" s="2">
@@ -3158,49 +2877,42 @@
       <c r="L40" s="1">
         <v>43607</v>
       </c>
-      <c r="M40" s="6">
-        <v>1</v>
+      <c r="M40" s="7">
+        <v>2</v>
       </c>
       <c r="N40" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O40">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P40">
         <v>19052201</v>
       </c>
       <c r="Q40" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>39_19052201</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="6">
-        <v>34</v>
-      </c>
+        <f t="shared" ref="Q40:Q57" si="2">CONCATENATE(O40,"_",P40)</f>
+        <v>40_19052201</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E41" s="2">
-        <v>43607</v>
-      </c>
+      <c r="C41" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="2"/>
       <c r="F41" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G41" s="7">
-        <v>8</v>
-      </c>
-      <c r="H41" s="7">
-        <v>8</v>
-      </c>
-      <c r="I41" s="6" t="s">
+      <c r="G41" s="6">
+        <v>9</v>
+      </c>
+      <c r="H41" s="6">
+        <v>9</v>
+      </c>
+      <c r="I41" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J41" s="2">
@@ -3212,39 +2924,32 @@
       <c r="L41" s="1">
         <v>43607</v>
       </c>
-      <c r="M41" s="7">
-        <v>2</v>
+      <c r="M41" s="6">
+        <v>1</v>
       </c>
       <c r="N41" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O41">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P41">
         <v>19052201</v>
       </c>
       <c r="Q41" s="6" t="str">
-        <f t="shared" ref="Q41:Q58" si="2">CONCATENATE(O41,"_",P41)</f>
-        <v>40_19052201</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="6">
-        <v>34</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>41_19052201</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E42" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="2"/>
       <c r="F42" s="6" t="s">
         <v>18</v>
       </c>
@@ -3254,7 +2959,7 @@
       <c r="H42" s="6">
         <v>9</v>
       </c>
-      <c r="I42" s="7" t="s">
+      <c r="I42" s="6" t="s">
         <v>21</v>
       </c>
       <c r="J42" s="2">
@@ -3267,48 +2972,41 @@
         <v>43607</v>
       </c>
       <c r="M42" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N42" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O42">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P42">
         <v>19052201</v>
       </c>
       <c r="Q42" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>41_19052201</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="6">
-        <v>34</v>
-      </c>
+        <v>42_19052201</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D43" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E43" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="2"/>
       <c r="F43" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G43" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H43" s="6">
-        <v>9</v>
-      </c>
-      <c r="I43" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J43" s="2">
@@ -3321,38 +3019,31 @@
         <v>43607</v>
       </c>
       <c r="M43" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N43" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O43">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P43">
         <v>19052201</v>
       </c>
       <c r="Q43" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>42_19052201</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="6">
-        <v>34</v>
-      </c>
+        <v>43_19052201</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D44" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E44" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="2"/>
       <c r="F44" s="6" t="s">
         <v>18</v>
       </c>
@@ -3362,7 +3053,7 @@
       <c r="H44" s="6">
         <v>10</v>
       </c>
-      <c r="I44" s="7" t="s">
+      <c r="I44" s="6" t="s">
         <v>21</v>
       </c>
       <c r="J44" s="2">
@@ -3375,48 +3066,41 @@
         <v>43607</v>
       </c>
       <c r="M44" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N44" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O44">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="P44">
         <v>19052201</v>
       </c>
       <c r="Q44" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>43_19052201</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="6">
-        <v>34</v>
-      </c>
+        <v>44_19052201</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D45" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E45" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="2"/>
       <c r="F45" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G45" s="6">
-        <v>10</v>
+        <v>11.5</v>
       </c>
       <c r="H45" s="6">
-        <v>10</v>
-      </c>
-      <c r="I45" s="6" t="s">
+        <v>11.5</v>
+      </c>
+      <c r="I45" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J45" s="2">
@@ -3429,38 +3113,31 @@
         <v>43607</v>
       </c>
       <c r="M45" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N45" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O45">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P45">
         <v>19052201</v>
       </c>
       <c r="Q45" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>44_19052201</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="6">
-        <v>34</v>
-      </c>
+        <v>45_19052201</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D46" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E46" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="2"/>
       <c r="F46" s="6" t="s">
         <v>18</v>
       </c>
@@ -3470,7 +3147,7 @@
       <c r="H46" s="6">
         <v>11.5</v>
       </c>
-      <c r="I46" s="7" t="s">
+      <c r="I46" s="6" t="s">
         <v>21</v>
       </c>
       <c r="J46" s="2">
@@ -3483,49 +3160,42 @@
         <v>43607</v>
       </c>
       <c r="M46" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N46" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O46">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P46">
         <v>19052201</v>
       </c>
       <c r="Q46" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>45_19052201</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="6">
-        <v>34</v>
-      </c>
+        <v>46_19052201</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E47" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="2"/>
       <c r="F47" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G47" s="6">
-        <v>11.5</v>
+        <v>2.5</v>
       </c>
       <c r="H47" s="6">
-        <v>11.5</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>21</v>
+        <v>2.5</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="J47" s="2">
         <v>43607</v>
@@ -3537,38 +3207,31 @@
         <v>43607</v>
       </c>
       <c r="M47" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N47" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O47">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P47">
         <v>19052201</v>
       </c>
       <c r="Q47" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>46_19052201</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="6">
-        <v>34</v>
-      </c>
+        <v>47_19052201</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E48" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="2"/>
       <c r="F48" s="6" t="s">
         <v>18</v>
       </c>
@@ -3578,7 +3241,7 @@
       <c r="H48" s="6">
         <v>2.5</v>
       </c>
-      <c r="I48" s="7" t="s">
+      <c r="I48" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J48" s="2">
@@ -3591,48 +3254,41 @@
         <v>43607</v>
       </c>
       <c r="M48" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N48" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O48">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P48">
         <v>19052201</v>
       </c>
       <c r="Q48" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>47_19052201</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="6">
-        <v>34</v>
-      </c>
+        <v>48_19052201</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E49" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="2"/>
       <c r="F49" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G49" s="6">
-        <v>2.5</v>
+        <v>9</v>
       </c>
       <c r="H49" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="I49" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I49" s="7" t="s">
         <v>30</v>
       </c>
       <c r="J49" s="2">
@@ -3645,38 +3301,31 @@
         <v>43607</v>
       </c>
       <c r="M49" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N49" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O49">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P49">
         <v>19052201</v>
       </c>
       <c r="Q49" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>48_19052201</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="6">
-        <v>34</v>
-      </c>
+        <v>49_19052201</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D50" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E50" s="2">
-        <v>43607</v>
-      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="2"/>
       <c r="F50" s="6" t="s">
         <v>18</v>
       </c>
@@ -3686,7 +3335,7 @@
       <c r="H50" s="6">
         <v>9</v>
       </c>
-      <c r="I50" s="7" t="s">
+      <c r="I50" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J50" s="2">
@@ -3699,49 +3348,40 @@
         <v>43607</v>
       </c>
       <c r="M50" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N50" s="6" t="s">
         <v>31</v>
       </c>
       <c r="O50">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P50">
         <v>19052201</v>
       </c>
       <c r="Q50" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>49_19052201</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="6">
-        <v>34</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E51" s="2">
-        <v>43607</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G51" s="6">
-        <v>9</v>
-      </c>
-      <c r="H51" s="6">
-        <v>9</v>
-      </c>
-      <c r="I51" s="6" t="s">
-        <v>30</v>
+        <v>50_19052201</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" t="s">
+        <v>17</v>
       </c>
       <c r="J51" s="2">
         <v>43607</v>
@@ -3752,93 +3392,75 @@
       <c r="L51" s="1">
         <v>43607</v>
       </c>
-      <c r="M51" s="6">
+      <c r="M51">
+        <v>3</v>
+      </c>
+      <c r="N51" t="s">
+        <v>31</v>
+      </c>
+      <c r="O51">
+        <v>51</v>
+      </c>
+      <c r="P51">
+        <v>19052201</v>
+      </c>
+      <c r="Q51" t="str">
+        <f t="shared" si="2"/>
+        <v>51_19052201</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" t="s">
+        <v>24</v>
+      </c>
+      <c r="J52" s="2">
+        <v>43607</v>
+      </c>
+      <c r="K52" t="s">
+        <v>33</v>
+      </c>
+      <c r="L52" s="1">
+        <v>43607</v>
+      </c>
+      <c r="M52">
         <v>2</v>
       </c>
-      <c r="N51" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="O51">
-        <v>50</v>
-      </c>
-      <c r="P51">
-        <v>19052201</v>
-      </c>
-      <c r="Q51" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>50_19052201</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>34</v>
-      </c>
-      <c r="B52" t="s">
-        <v>16</v>
-      </c>
-      <c r="C52" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E52" s="2">
-        <v>43607</v>
-      </c>
-      <c r="F52" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" t="s">
-        <v>16</v>
-      </c>
-      <c r="H52" t="s">
-        <v>16</v>
-      </c>
-      <c r="I52" t="s">
-        <v>17</v>
-      </c>
-      <c r="J52" s="2">
-        <v>43607</v>
-      </c>
-      <c r="K52" t="s">
-        <v>33</v>
-      </c>
-      <c r="L52" s="1">
-        <v>43607</v>
-      </c>
-      <c r="M52">
-        <v>3</v>
-      </c>
       <c r="N52" t="s">
         <v>31</v>
       </c>
       <c r="O52">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P52">
         <v>19052201</v>
       </c>
       <c r="Q52" t="str">
         <f t="shared" si="2"/>
-        <v>51_19052201</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>34</v>
-      </c>
+        <v>52_19052201</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>16</v>
       </c>
       <c r="C53" t="s">
         <v>16</v>
       </c>
-      <c r="D53" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E53" s="2">
-        <v>43607</v>
-      </c>
       <c r="F53" t="s">
         <v>16</v>
       </c>
@@ -3849,7 +3471,7 @@
         <v>16</v>
       </c>
       <c r="I53" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J53" s="2">
         <v>43607</v>
@@ -3867,32 +3489,23 @@
         <v>31</v>
       </c>
       <c r="O53">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P53">
         <v>19052201</v>
       </c>
       <c r="Q53" t="str">
         <f t="shared" si="2"/>
-        <v>52_19052201</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>34</v>
-      </c>
+        <v>53_19052201</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>16</v>
       </c>
       <c r="C54" t="s">
         <v>16</v>
       </c>
-      <c r="D54" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E54" s="2">
-        <v>43607</v>
-      </c>
       <c r="F54" t="s">
         <v>16</v>
       </c>
@@ -3903,7 +3516,7 @@
         <v>16</v>
       </c>
       <c r="I54" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J54" s="2">
         <v>43607</v>
@@ -3921,32 +3534,23 @@
         <v>31</v>
       </c>
       <c r="O54">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P54">
         <v>19052201</v>
       </c>
       <c r="Q54" t="str">
         <f t="shared" si="2"/>
-        <v>53_19052201</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>34</v>
-      </c>
+        <v>54_19052201</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>16</v>
       </c>
       <c r="C55" t="s">
         <v>16</v>
       </c>
-      <c r="D55" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E55" s="2">
-        <v>43607</v>
-      </c>
       <c r="F55" t="s">
         <v>16</v>
       </c>
@@ -3957,7 +3561,7 @@
         <v>16</v>
       </c>
       <c r="I55" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J55" s="2">
         <v>43607</v>
@@ -3975,32 +3579,23 @@
         <v>31</v>
       </c>
       <c r="O55">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P55">
         <v>19052201</v>
       </c>
       <c r="Q55" t="str">
         <f t="shared" si="2"/>
-        <v>54_19052201</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>34</v>
-      </c>
+        <v>55_19052201</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>16</v>
       </c>
       <c r="C56" t="s">
         <v>16</v>
       </c>
-      <c r="D56" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E56" s="2">
-        <v>43607</v>
-      </c>
       <c r="F56" t="s">
         <v>16</v>
       </c>
@@ -4011,7 +3606,7 @@
         <v>16</v>
       </c>
       <c r="I56" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J56" s="2">
         <v>43607</v>
@@ -4029,32 +3624,23 @@
         <v>31</v>
       </c>
       <c r="O56">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P56">
         <v>19052201</v>
       </c>
       <c r="Q56" t="str">
         <f t="shared" si="2"/>
-        <v>55_19052201</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>34</v>
-      </c>
+        <v>56_19052201</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>16</v>
       </c>
       <c r="C57" t="s">
         <v>16</v>
       </c>
-      <c r="D57" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E57" s="2">
-        <v>43607</v>
-      </c>
       <c r="F57" t="s">
         <v>16</v>
       </c>
@@ -4065,7 +3651,7 @@
         <v>16</v>
       </c>
       <c r="I57" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="J57" s="2">
         <v>43607</v>
@@ -4077,72 +3663,18 @@
         <v>43607</v>
       </c>
       <c r="M57">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N57" t="s">
         <v>31</v>
       </c>
       <c r="O57">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="P57">
         <v>19052201</v>
       </c>
       <c r="Q57" t="str">
-        <f t="shared" si="2"/>
-        <v>56_19052201</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>34</v>
-      </c>
-      <c r="B58" t="s">
-        <v>16</v>
-      </c>
-      <c r="C58" t="s">
-        <v>16</v>
-      </c>
-      <c r="D58" s="1">
-        <v>43607</v>
-      </c>
-      <c r="E58" s="2">
-        <v>43607</v>
-      </c>
-      <c r="F58" t="s">
-        <v>16</v>
-      </c>
-      <c r="G58" t="s">
-        <v>16</v>
-      </c>
-      <c r="H58" t="s">
-        <v>16</v>
-      </c>
-      <c r="I58" t="s">
-        <v>17</v>
-      </c>
-      <c r="J58" s="2">
-        <v>43607</v>
-      </c>
-      <c r="K58" t="s">
-        <v>33</v>
-      </c>
-      <c r="L58" s="1">
-        <v>43607</v>
-      </c>
-      <c r="M58">
-        <v>4</v>
-      </c>
-      <c r="N58" t="s">
-        <v>31</v>
-      </c>
-      <c r="O58">
-        <v>57</v>
-      </c>
-      <c r="P58">
-        <v>19052201</v>
-      </c>
-      <c r="Q58" t="str">
         <f t="shared" si="2"/>
         <v>57_19052201</v>
       </c>

</xml_diff>